<commit_message>
Update iteration2 docs, remove app.iml again
</commit_message>
<xml_diff>
--- a/Documentation/Itr2/Software Engineering 7 - Group Log.xlsx.xlsx
+++ b/Documentation/Itr2/Software Engineering 7 - Group Log.xlsx.xlsx
@@ -18,7 +18,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="I23">
+    <comment authorId="0" ref="I26">
       <text>
         <t xml:space="preserve">Lam: Duplicate?
 	-Paul Jarrow</t>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="166">
   <si>
     <t>When</t>
   </si>
@@ -193,105 +193,135 @@
     <t>branch: task-item-add-fixes</t>
   </si>
   <si>
-    <t>Finalized removeTask() method and got it to work</t>
+    <t>3hours</t>
+  </si>
+  <si>
+    <t>Alarms</t>
+  </si>
+  <si>
+    <t>Research on alarms</t>
+  </si>
+  <si>
+    <t>Xiran</t>
+  </si>
+  <si>
+    <t>Finalized removeTask() method</t>
+  </si>
+  <si>
+    <t>7.5 hours</t>
+  </si>
+  <si>
+    <t>Add Alarm</t>
+  </si>
+  <si>
+    <t>Allowing user to add alarm for each task</t>
+  </si>
+  <si>
+    <t>Researching and implementing alarms on local branch</t>
+  </si>
+  <si>
+    <t>Researched how to implementing alarms</t>
+  </si>
+  <si>
+    <t>Finalized removeTask() method and got it to work -&gt; Working for real this time</t>
+  </si>
+  <si>
+    <t>Priorities</t>
+  </si>
+  <si>
+    <t>Reaseached and implemented spinners on local branch</t>
+  </si>
+  <si>
+    <t>4.5 hours</t>
+  </si>
+  <si>
+    <t>Item Priorities</t>
+  </si>
+  <si>
+    <t>Changing priority ranking of an individual item</t>
+  </si>
+  <si>
+    <t>Researching spinner objects for priority implementation</t>
+  </si>
+  <si>
+    <t>Draw user interface for Priority User Story</t>
+  </si>
+  <si>
+    <t>7 hours</t>
+  </si>
+  <si>
+    <t>Implementing UI and Class for prirority spinner</t>
+  </si>
+  <si>
+    <t>implementing spinner for item priorities</t>
+  </si>
+  <si>
+    <t>Reaseached how to fix bug (The program will crash while editing task and clicking Delete task)</t>
+  </si>
+  <si>
+    <t>Priorities DB</t>
+  </si>
+  <si>
+    <t>Structure and database implementation for priorities</t>
+  </si>
+  <si>
+    <t>Please see https://github.com/DotFreelance/To-Do-Bot/wiki/Paul-J:-Changelog</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>Trying to fix the resolution for the priorities pictures</t>
+  </si>
+  <si>
+    <t>Setting item piorities and organizing items based on priorites</t>
+  </si>
+  <si>
+    <t>Priorities cleanup</t>
+  </si>
+  <si>
+    <t>Priorities cleanup: fixed mipmaps for priorities, fixed bugs</t>
+  </si>
+  <si>
+    <t>1.5 hours</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Finished leftover testing from iteration 1</t>
+  </si>
+  <si>
+    <t>Iteration 3 Starts - March 14th, 2016</t>
+  </si>
+  <si>
+    <t>Where</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Attendees</t>
+  </si>
+  <si>
+    <t>E2 tables</t>
+  </si>
+  <si>
+    <t>- Set up Slack and Asana</t>
+  </si>
+  <si>
+    <t>- Planned the next meeting</t>
+  </si>
+  <si>
+    <t>- Came up with ideas for the apps: to-do list or expense tracking</t>
   </si>
   <si>
     <t>Lam</t>
   </si>
   <si>
-    <t>7.5 hours</t>
-  </si>
-  <si>
-    <t>Add Alarm</t>
-  </si>
-  <si>
-    <t>Allowing user to add alarm for each task</t>
-  </si>
-  <si>
-    <t>Researching and implementing alarms on local branch</t>
-  </si>
-  <si>
-    <t>Alarms</t>
-  </si>
-  <si>
-    <t>Researched how to implementing alarms</t>
-  </si>
-  <si>
-    <t>Finalized removeTask() method and got it to work -&gt; Working for real this time</t>
-  </si>
-  <si>
-    <t>Priorities</t>
-  </si>
-  <si>
-    <t>Reaseached and implemented spinners on local branch</t>
-  </si>
-  <si>
-    <t>4.5 hours</t>
-  </si>
-  <si>
-    <t>Item Priorities</t>
-  </si>
-  <si>
-    <t>Changing priority ranking of an individual item</t>
-  </si>
-  <si>
-    <t>Researching spinner objects for priority implementation</t>
-  </si>
-  <si>
-    <t>implementing spinner for item priorities</t>
-  </si>
-  <si>
-    <t>Priorities DB</t>
-  </si>
-  <si>
-    <t>Structure and database implementation for priorities</t>
-  </si>
-  <si>
-    <t>Please see https://github.com/DotFreelance/To-Do-Bot/wiki/Paul-J:-Changelog</t>
-  </si>
-  <si>
-    <t>2 hours</t>
-  </si>
-  <si>
-    <t>Setting item piorities and organizing items based on priorites</t>
-  </si>
-  <si>
-    <t>Priorities cleanup</t>
-  </si>
-  <si>
-    <t>Priorities cleanup: fixed mipmaps for priorities, fixed bugs</t>
-  </si>
-  <si>
-    <t>Iteration 3 Starts - March 14th, 2016</t>
-  </si>
-  <si>
-    <t>Where</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Attendees</t>
-  </si>
-  <si>
-    <t>E2 tables</t>
-  </si>
-  <si>
-    <t>- Set up Slack and Asana</t>
-  </si>
-  <si>
-    <t>- Planned the next meeting</t>
-  </si>
-  <si>
-    <t>- Came up with ideas for the apps: to-do list or expense tracking</t>
-  </si>
-  <si>
-    <t>Xiran</t>
-  </si>
-  <si>
     <t>- Looked for potential customers</t>
   </si>
   <si>
@@ -430,6 +460,9 @@
     <t>Room 223A</t>
   </si>
   <si>
+    <t>- Finished off iteration 2</t>
+  </si>
+  <si>
     <t>Upcoming Meetings</t>
   </si>
   <si>
@@ -476,6 +509,9 @@
   </si>
   <si>
     <t>Monday, March 28, 2016</t>
+  </si>
+  <si>
+    <t>Room 360</t>
   </si>
   <si>
     <t>Wednesday, March 30, 2016</t>
@@ -1037,60 +1073,58 @@
     </row>
     <row r="16">
       <c r="A16" s="15">
-        <v>42438.0</v>
+        <v>42434.0</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="14" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>49</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H16" s="14"/>
     </row>
     <row r="17">
       <c r="A17" s="15">
-        <v>42439.0</v>
-      </c>
-      <c r="B17" s="16">
-        <v>0.8125</v>
-      </c>
-      <c r="C17" s="16">
-        <v>0.125</v>
-      </c>
+        <v>42438.0</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
       <c r="D17" s="14" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>58</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="15">
         <v>42439.0</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
+      <c r="B18" s="16">
+        <v>0.8125</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0.125</v>
+      </c>
       <c r="D18" s="14" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>60</v>
@@ -1099,43 +1133,43 @@
         <v>61</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="11"/>
+        <v>40</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="15">
         <v>42439.0</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="14" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="14" t="s">
-        <v>49</v>
-      </c>
+      <c r="H19" s="11"/>
     </row>
     <row r="20">
       <c r="A20" s="15">
-        <v>42440.0</v>
+        <v>42439.0</v>
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="D20" s="14" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>64</v>
@@ -1143,49 +1177,45 @@
       <c r="G20" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="14"/>
+      <c r="H20" s="14" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="15">
         <v>42440.0</v>
       </c>
-      <c r="B21" s="16">
-        <v>0.9375</v>
-      </c>
-      <c r="C21" s="16">
-        <v>0.125</v>
-      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="F21" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>67</v>
-      </c>
       <c r="G21" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>68</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="H21" s="14"/>
     </row>
     <row r="22">
       <c r="A22" s="15">
-        <v>42441.0</v>
+        <v>42440.0</v>
       </c>
       <c r="B22" s="16">
-        <v>0.9166666666666666</v>
+        <v>0.9375</v>
       </c>
       <c r="C22" s="16">
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>69</v>
@@ -1193,66 +1223,69 @@
       <c r="G22" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="11"/>
+      <c r="H22" s="14" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="15">
-        <v>42441.0</v>
+        <v>42440.0</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="14" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="13"/>
+        <v>26</v>
+      </c>
+      <c r="H23" s="14"/>
     </row>
     <row r="24">
       <c r="A24" s="15">
-        <v>42441.0</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
+        <v>42440.0</v>
+      </c>
+      <c r="B24" s="16">
+        <v>0.875</v>
+      </c>
+      <c r="C24" s="16">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="D24" s="14" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>72</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H24" s="11"/>
     </row>
     <row r="25">
       <c r="A25" s="15">
-        <v>42442.0</v>
+        <v>42441.0</v>
       </c>
       <c r="B25" s="16">
-        <v>0.625</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="C25" s="16">
-        <v>0.7083333333333334</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>74</v>
@@ -1264,89 +1297,152 @@
     </row>
     <row r="26">
       <c r="A26" s="15">
-        <v>42442.0</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+        <v>42441.0</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="14" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="E26" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="14" t="s">
-        <v>76</v>
-      </c>
       <c r="G26" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>72</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="I26" s="13"/>
     </row>
     <row r="27">
+      <c r="A27" s="15">
+        <v>42441.0</v>
+      </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
+      <c r="D27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
-        <v>77</v>
-      </c>
+      <c r="A28" s="15">
+        <v>42442.0</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="11"/>
     </row>
     <row r="29">
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
+      <c r="A29" s="15">
+        <v>42442.0</v>
+      </c>
+      <c r="B29" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="C29" s="16">
+        <v>0.7083333333333334</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>40</v>
+      </c>
       <c r="H29" s="11"/>
     </row>
     <row r="30">
+      <c r="A30" s="15">
+        <v>42442.0</v>
+      </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
+      <c r="D30" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="31">
+      <c r="A31" s="15">
+        <v>42443.0</v>
+      </c>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
+      <c r="D31" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>16</v>
+      </c>
       <c r="H31" s="11"/>
     </row>
     <row r="32">
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
     </row>
     <row r="33">
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
+      <c r="A33" s="17" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
+      <c r="D34" s="14"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -10108,6 +10204,51 @@
       <c r="F1007" s="11"/>
       <c r="G1007" s="11"/>
       <c r="H1007" s="11"/>
+    </row>
+    <row r="1008">
+      <c r="B1008" s="11"/>
+      <c r="C1008" s="11"/>
+      <c r="D1008" s="11"/>
+      <c r="E1008" s="11"/>
+      <c r="F1008" s="11"/>
+      <c r="G1008" s="11"/>
+      <c r="H1008" s="11"/>
+    </row>
+    <row r="1009">
+      <c r="B1009" s="11"/>
+      <c r="C1009" s="11"/>
+      <c r="D1009" s="11"/>
+      <c r="E1009" s="11"/>
+      <c r="F1009" s="11"/>
+      <c r="G1009" s="11"/>
+      <c r="H1009" s="11"/>
+    </row>
+    <row r="1010">
+      <c r="B1010" s="11"/>
+      <c r="C1010" s="11"/>
+      <c r="D1010" s="11"/>
+      <c r="E1010" s="11"/>
+      <c r="F1010" s="11"/>
+      <c r="G1010" s="11"/>
+      <c r="H1010" s="11"/>
+    </row>
+    <row r="1011">
+      <c r="B1011" s="11"/>
+      <c r="C1011" s="11"/>
+      <c r="D1011" s="11"/>
+      <c r="E1011" s="11"/>
+      <c r="F1011" s="11"/>
+      <c r="G1011" s="11"/>
+      <c r="H1011" s="11"/>
+    </row>
+    <row r="1012">
+      <c r="B1012" s="11"/>
+      <c r="C1012" s="11"/>
+      <c r="D1012" s="11"/>
+      <c r="E1012" s="11"/>
+      <c r="F1012" s="11"/>
+      <c r="G1012" s="11"/>
+      <c r="H1012" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -10118,7 +10259,7 @@
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A33:H33"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:C2"/>
@@ -10150,7 +10291,7 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="18" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>1</v>
@@ -10173,13 +10314,13 @@
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="19" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" ht="16.5" customHeight="1">
@@ -10210,10 +10351,10 @@
         <v>0.6458333333333334</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="F4" s="25" t="s">
         <v>26</v>
@@ -10234,7 +10375,7 @@
       <c r="C5" s="27"/>
       <c r="D5" s="23"/>
       <c r="E5" s="24" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="28"/>
@@ -10267,10 +10408,10 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="F7" s="25" t="s">
         <v>26</v>
@@ -10279,10 +10420,10 @@
         <v>33</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
@@ -10293,7 +10434,7 @@
       <c r="C8" s="27"/>
       <c r="D8" s="23"/>
       <c r="E8" s="24" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="28"/>
@@ -10308,7 +10449,7 @@
       <c r="C9" s="27"/>
       <c r="D9" s="23"/>
       <c r="E9" s="24" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="28"/>
@@ -10341,10 +10482,10 @@
         <v>0.7083333333333334</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F11" s="25" t="s">
         <v>26</v>
@@ -10353,10 +10494,10 @@
         <v>33</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="J11" s="26"/>
       <c r="K11" s="26"/>
@@ -10367,7 +10508,7 @@
       <c r="C12" s="27"/>
       <c r="D12" s="23"/>
       <c r="E12" s="24" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="28"/>
@@ -10382,7 +10523,7 @@
       <c r="C13" s="27"/>
       <c r="D13" s="23"/>
       <c r="E13" s="24" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="28"/>
@@ -10397,7 +10538,7 @@
       <c r="C14" s="27"/>
       <c r="D14" s="23"/>
       <c r="E14" s="24" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="28"/>
@@ -10412,7 +10553,7 @@
       <c r="C15" s="27"/>
       <c r="D15" s="23"/>
       <c r="E15" s="24" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="F15" s="25"/>
       <c r="G15" s="28"/>
@@ -10427,7 +10568,7 @@
       <c r="C16" s="27"/>
       <c r="D16" s="23"/>
       <c r="E16" s="24" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="28"/>
@@ -10460,10 +10601,10 @@
         <v>0.7291666666666666</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="F18" s="25" t="s">
         <v>26</v>
@@ -10472,10 +10613,10 @@
         <v>33</v>
       </c>
       <c r="H18" s="29" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="J18" s="30" t="s">
         <v>40</v>
@@ -10490,7 +10631,7 @@
       <c r="C19" s="27"/>
       <c r="D19" s="23"/>
       <c r="E19" s="24" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="28"/>
@@ -10523,10 +10664,10 @@
         <v>0.71875</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="F21" s="25" t="s">
         <v>26</v>
@@ -10535,10 +10676,10 @@
         <v>33</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I21" s="28" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="J21" s="30" t="s">
         <v>40</v>
@@ -10551,7 +10692,7 @@
       <c r="C22" s="27"/>
       <c r="D22" s="23"/>
       <c r="E22" s="31" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="28"/>
@@ -10584,10 +10725,10 @@
         <v>0.71875</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="F24" s="25" t="s">
         <v>26</v>
@@ -10596,10 +10737,10 @@
         <v>33</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I24" s="28" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="J24" s="30" t="s">
         <v>40</v>
@@ -10612,7 +10753,7 @@
       <c r="C25" s="27"/>
       <c r="D25" s="23"/>
       <c r="E25" s="13" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F25" s="25"/>
       <c r="G25" s="28"/>
@@ -10627,7 +10768,7 @@
       <c r="C26" s="27"/>
       <c r="D26" s="23"/>
       <c r="E26" s="13" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="F26" s="25"/>
       <c r="G26" s="28"/>
@@ -10642,7 +10783,7 @@
       <c r="C27" s="27"/>
       <c r="D27" s="23"/>
       <c r="E27" s="32" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="F27" s="25"/>
       <c r="G27" s="28"/>
@@ -10675,10 +10816,10 @@
         <v>0.71875</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E29" s="34" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="F29" s="25" t="s">
         <v>26</v>
@@ -10688,7 +10829,7 @@
       </c>
       <c r="H29" s="29"/>
       <c r="I29" s="28" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="J29" s="30" t="s">
         <v>40</v>
@@ -10721,10 +10862,10 @@
         <v>0.71875</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E31" s="36" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="F31" s="25" t="s">
         <v>26</v>
@@ -10733,10 +10874,10 @@
         <v>33</v>
       </c>
       <c r="H31" s="29" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I31" s="28" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="J31" s="30" t="s">
         <v>40</v>
@@ -10751,7 +10892,7 @@
       <c r="C32" s="35"/>
       <c r="D32" s="23"/>
       <c r="E32" s="36" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="F32" s="25"/>
       <c r="G32" s="28"/>
@@ -10766,7 +10907,7 @@
       <c r="C33" s="35"/>
       <c r="D33" s="23"/>
       <c r="E33" s="36" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="F33" s="25"/>
       <c r="G33" s="28"/>
@@ -10798,20 +10939,20 @@
         <v>0.71875</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="F35" s="25" t="s">
         <v>26</v>
       </c>
       <c r="G35" s="28"/>
       <c r="H35" s="29" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I35" s="28" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="J35" s="30" t="s">
         <v>40</v>
@@ -10844,10 +10985,10 @@
         <v>0.75</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E37" s="36" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="F37" s="25" t="s">
         <v>26</v>
@@ -10856,10 +10997,10 @@
         <v>33</v>
       </c>
       <c r="H37" s="29" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I37" s="28" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="J37" s="30" t="s">
         <v>40</v>
@@ -10872,7 +11013,7 @@
       <c r="C38" s="35"/>
       <c r="D38" s="25"/>
       <c r="E38" s="36" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="F38" s="25"/>
       <c r="G38" s="26"/>
@@ -10887,7 +11028,7 @@
       <c r="C39" s="35"/>
       <c r="D39" s="25"/>
       <c r="E39" s="36" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="26"/>
@@ -10902,7 +11043,7 @@
       <c r="C40" s="35"/>
       <c r="D40" s="25"/>
       <c r="E40" s="36" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="F40" s="25"/>
       <c r="G40" s="26"/>
@@ -10917,7 +11058,7 @@
       <c r="C41" s="35"/>
       <c r="D41" s="25"/>
       <c r="E41" s="34" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="F41" s="25"/>
       <c r="G41" s="26"/>
@@ -10950,10 +11091,10 @@
         <v>0.7291666666666666</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="F43" s="23" t="s">
         <v>26</v>
@@ -10962,7 +11103,7 @@
         <v>33</v>
       </c>
       <c r="H43" s="30" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I43" s="30"/>
       <c r="J43" s="30" t="s">
@@ -10976,7 +11117,7 @@
       <c r="C44" s="35"/>
       <c r="D44" s="25"/>
       <c r="E44" s="36" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="F44" s="33"/>
     </row>
@@ -10986,7 +11127,7 @@
       <c r="C45" s="35"/>
       <c r="D45" s="25"/>
       <c r="E45" s="36" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="F45" s="33"/>
     </row>
@@ -11009,20 +11150,20 @@
         <v>0.7291666666666666</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E47" s="36" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="F47" s="24"/>
       <c r="G47" s="30" t="s">
         <v>33</v>
       </c>
       <c r="H47" s="30" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I47" s="30" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="J47" s="30" t="s">
         <v>40</v>
@@ -11037,7 +11178,7 @@
       <c r="C48" s="35"/>
       <c r="D48" s="25"/>
       <c r="E48" s="36" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="F48" s="33"/>
     </row>
@@ -11060,10 +11201,10 @@
         <v>0.7291666666666666</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E50" s="36" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="F50" s="23" t="s">
         <v>26</v>
@@ -11072,7 +11213,7 @@
         <v>33</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I50" s="26"/>
       <c r="J50" s="30" t="s">
@@ -11098,20 +11239,20 @@
         <v>0.7291666666666666</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="F52" s="33"/>
       <c r="G52" s="30" t="s">
         <v>33</v>
       </c>
       <c r="H52" s="30" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I52" s="30" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="J52" s="30" t="s">
         <v>40</v>
@@ -11123,7 +11264,7 @@
       <c r="C53" s="35"/>
       <c r="D53" s="25"/>
       <c r="E53" s="24" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="F53" s="33"/>
     </row>
@@ -11133,7 +11274,7 @@
       <c r="C54" s="35"/>
       <c r="D54" s="25"/>
       <c r="E54" s="24" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="F54" s="33"/>
     </row>
@@ -11143,7 +11284,7 @@
       <c r="C55" s="35"/>
       <c r="D55" s="25"/>
       <c r="E55" s="24" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="F55" s="33"/>
     </row>
@@ -11153,7 +11294,7 @@
       <c r="C56" s="35"/>
       <c r="D56" s="25"/>
       <c r="E56" s="24" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="F56" s="33"/>
     </row>
@@ -11176,10 +11317,10 @@
         <v>0.7291666666666666</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E58" s="24" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="F58" s="23" t="s">
         <v>26</v>
@@ -11188,10 +11329,10 @@
         <v>33</v>
       </c>
       <c r="H58" s="30" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I58" s="30" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="J58" s="30" t="s">
         <v>40</v>
@@ -11200,21 +11341,21 @@
     <row r="59">
       <c r="D59" s="25"/>
       <c r="E59" s="24" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="F59" s="33"/>
     </row>
     <row r="60">
       <c r="D60" s="25"/>
       <c r="E60" s="24" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="F60" s="33"/>
     </row>
     <row r="61">
       <c r="D61" s="25"/>
       <c r="E61" s="24" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="F61" s="33"/>
     </row>
@@ -11234,9 +11375,11 @@
         <v>0.7291666666666666</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="E63" s="33"/>
+        <v>142</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>143</v>
+      </c>
       <c r="F63" s="23" t="s">
         <v>26</v>
       </c>
@@ -11244,10 +11387,10 @@
         <v>33</v>
       </c>
       <c r="H63" s="30" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="I63" s="30" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="J63" s="30" t="s">
         <v>40</v>
@@ -16070,7 +16213,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="40" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -16079,30 +16222,30 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D3" s="39">
         <v>0.6041666666666666</v>
@@ -16113,13 +16256,13 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D4" s="39">
         <v>0.6041666666666666</v>
@@ -16130,13 +16273,13 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>132</v>
-      </c>
       <c r="C5" s="13" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D5" s="39">
         <v>0.6041666666666666</v>
@@ -16147,13 +16290,13 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D6" s="39">
         <v>0.6041666666666666</v>
@@ -16164,13 +16307,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D7" s="39">
         <v>0.6041666666666666</v>
@@ -16181,13 +16324,13 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D8" s="39">
         <v>0.6041666666666666</v>
@@ -16198,7 +16341,13 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>148</v>
+        <v>159</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>151</v>
       </c>
       <c r="D9" s="39">
         <v>0.6041666666666666</v>
@@ -16209,7 +16358,7 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="D10" s="39">
         <v>0.6041666666666666</v>
@@ -16220,7 +16369,7 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="D11" s="39">
         <v>0.6041666666666666</v>
@@ -16231,7 +16380,7 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="D12" s="39">
         <v>0.6041666666666666</v>
@@ -16242,7 +16391,7 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="D13" s="39">
         <v>0.6041666666666666</v>
@@ -16253,7 +16402,7 @@
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="D14" s="39">
         <v>0.6041666666666666</v>

</xml_diff>